<commit_message>
ADD: add simpleLayeredTexture to regression test
Former-commit-id: 1d9e25df476d49d19ffbaa363183e2e905380c5b
</commit_message>
<xml_diff>
--- a/tests/cuda4.1sdk/regression/llvm_status.xlsx
+++ b/tests/cuda4.1sdk/regression/llvm_status.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
   <si>
     <t>PassFail</t>
   </si>
@@ -209,6 +209,12 @@
     <t>RadixSortThrust</t>
   </si>
   <si>
+    <t>Use vote instruction</t>
+  </si>
+  <si>
+    <t>No / Ignored test</t>
+  </si>
+  <si>
     <t>RecursiveGaussian</t>
   </si>
   <si>
@@ -236,6 +242,15 @@
     <t>SimpleLayeredTexture</t>
   </si>
   <si>
+    <t>Did not complete / Pass</t>
+  </si>
+  <si>
+    <t>One texture instruction is not implemented</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>SimpleMPI</t>
   </si>
   <si>
@@ -297,9 +312,6 @@
   </si>
   <si>
     <t>The device function reduceBlock() Utilized the implicit warp synchronization. The way that LLVM backend executes kernel (by a loop preserving the explicity barrier) does not support it.</t>
-  </si>
-  <si>
-    <t>No / Ignored test</t>
   </si>
   <si>
     <t>ThreadMigration</t>
@@ -407,7 +419,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -418,6 +430,7 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -438,15 +451,15 @@
   <dimension ref="A1:T83"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="B58" activeCellId="0" pane="topLeft" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="17.3019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="17.3843137254902"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
@@ -460,7 +473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -469,7 +482,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
@@ -478,7 +491,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>7</v>
       </c>
@@ -487,7 +500,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -499,7 +512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>11</v>
       </c>
@@ -508,7 +521,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
@@ -517,7 +530,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
@@ -526,7 +539,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
@@ -535,7 +548,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>15</v>
       </c>
@@ -544,7 +557,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -556,7 +569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -568,7 +581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>20</v>
       </c>
@@ -577,7 +590,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>21</v>
       </c>
@@ -586,7 +599,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>22</v>
       </c>
@@ -595,7 +608,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -607,7 +620,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="17">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -619,7 +632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="18">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -628,7 +641,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>29</v>
       </c>
@@ -637,7 +650,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="20">
       <c r="A20" s="2" t="s">
         <v>30</v>
       </c>
@@ -649,7 +662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>31</v>
       </c>
@@ -658,7 +671,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>32</v>
       </c>
@@ -667,7 +680,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>33</v>
       </c>
@@ -676,7 +689,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="24">
       <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
@@ -688,7 +701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="25">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -700,7 +713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>36</v>
       </c>
@@ -709,7 +722,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="27">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -721,7 +734,7 @@
         <v>38</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>39</v>
       </c>
@@ -730,7 +743,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="57.45" outlineLevel="0" r="29">
       <c r="A29" s="3" t="s">
         <v>40</v>
       </c>
@@ -762,7 +775,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="30">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -790,7 +803,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="31">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
@@ -818,7 +831,7 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="32">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -846,7 +859,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="33">
       <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
@@ -874,7 +887,7 @@
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="34">
       <c r="A34" s="2" t="s">
         <v>49</v>
       </c>
@@ -902,7 +915,7 @@
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="35">
       <c r="A35" s="2" t="s">
         <v>50</v>
       </c>
@@ -911,7 +924,7 @@
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="36">
       <c r="A36" s="2" t="s">
         <v>51</v>
       </c>
@@ -920,7 +933,7 @@
       </c>
       <c r="D36" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>52</v>
       </c>
@@ -929,7 +942,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>53</v>
       </c>
@@ -938,7 +951,7 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>54</v>
       </c>
@@ -947,7 +960,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="40">
       <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
@@ -975,7 +988,7 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
         <v>56</v>
       </c>
@@ -984,7 +997,7 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="42">
       <c r="A42" s="2" t="s">
         <v>57</v>
       </c>
@@ -1012,7 +1025,7 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="43">
       <c r="A43" s="2" t="s">
         <v>58</v>
       </c>
@@ -1040,7 +1053,7 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="44">
       <c r="A44" s="2" t="s">
         <v>59</v>
       </c>
@@ -1068,7 +1081,7 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="45">
       <c r="A45" s="2" t="s">
         <v>60</v>
       </c>
@@ -1096,7 +1109,7 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="46">
       <c r="A46" s="2" t="s">
         <v>61</v>
       </c>
@@ -1105,7 +1118,7 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>62</v>
       </c>
@@ -1114,18 +1127,22 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="48">
       <c r="A48" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="2"/>
+      <c r="C48" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D48" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -1142,9 +1159,9 @@
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="49">
       <c r="A49" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>9</v>
@@ -1170,9 +1187,9 @@
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="50">
       <c r="A50" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>9</v>
@@ -1198,18 +1215,18 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="52">
       <c r="A52" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>9</v>
@@ -1235,9 +1252,9 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="53">
       <c r="A53" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>17</v>
@@ -1263,18 +1280,18 @@
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="55">
       <c r="A55" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>17</v>
@@ -1300,154 +1317,158 @@
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="57">
-      <c r="A57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C57" s="2"/>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="57" s="4">
+      <c r="A57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="D57" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="58">
+      <c r="E57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="58">
       <c r="A58" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="61">
       <c r="A61" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D61" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D63" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D64" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="65">
       <c r="A65" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D65" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D68" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="69">
       <c r="A69" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D69" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="70">
       <c r="A70" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>9</v>
@@ -1473,18 +1494,18 @@
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D71" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="72">
       <c r="A72" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>17</v>
@@ -1510,57 +1531,57 @@
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D73" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D75" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D76" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="124.6" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="124.6" outlineLevel="0" r="77">
       <c r="A77" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -1578,54 +1599,54 @@
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="78">
       <c r="A78" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D78" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>5</v>
       </c>
       <c r="D80" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="81">
       <c r="A81" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D81" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="82">
       <c r="A82" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D82" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>5</v>

</xml_diff>